<commit_message>
completed data for humann2 taxa
</commit_message>
<xml_diff>
--- a/prototypes/post-run-analysis/taxa_rpk_amalgam/mpro_final_taxa.xlsx
+++ b/prototypes/post-run-analysis/taxa_rpk_amalgam/mpro_final_taxa.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0E3742-BFAB-4094-A8D5-58D5B2DE2ABA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3989EF97-46BD-43F2-AF2B-ECD1507D7F87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>unmapped</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>humann2</t>
+  </si>
+  <si>
+    <t>mpro</t>
+  </si>
+  <si>
+    <t>wc</t>
+  </si>
+  <si>
+    <t>raw reads</t>
   </si>
 </sst>
 </file>
@@ -1463,16 +1475,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1763,72 +1775,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:AI14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="A2:C10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AG14" sqref="AG14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
       </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
       <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="W1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="X1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Y1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Z1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AA1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AC1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AD1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AE1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AF1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AG1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AH1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AI1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1836,55 +1891,91 @@
         <v>89.72</v>
       </c>
       <c r="C2">
-        <f>U2*100/V2</f>
+        <f>AG2*100/AH2</f>
         <v>72.181674772771458</v>
       </c>
+      <c r="F2">
+        <v>2164110</v>
+      </c>
+      <c r="G2">
+        <v>2421648</v>
+      </c>
+      <c r="H2">
+        <v>1088422</v>
+      </c>
       <c r="I2">
+        <v>2933606</v>
+      </c>
+      <c r="J2">
+        <v>1900477</v>
+      </c>
+      <c r="K2">
+        <v>1414049</v>
+      </c>
+      <c r="L2">
+        <v>2443977</v>
+      </c>
+      <c r="M2">
+        <v>1418697</v>
+      </c>
+      <c r="N2">
+        <v>2103262</v>
+      </c>
+      <c r="O2">
+        <v>2338975</v>
+      </c>
+      <c r="P2">
+        <v>3811278</v>
+      </c>
+      <c r="Q2">
+        <v>2026711</v>
+      </c>
+      <c r="U2">
         <v>511210</v>
       </c>
-      <c r="J2">
+      <c r="V2">
         <v>620147</v>
       </c>
-      <c r="K2">
+      <c r="W2">
         <v>320997</v>
       </c>
-      <c r="L2">
+      <c r="X2">
         <v>861832</v>
       </c>
-      <c r="M2">
+      <c r="Y2">
         <v>417937</v>
       </c>
-      <c r="N2">
+      <c r="Z2">
         <v>541742</v>
       </c>
-      <c r="O2">
+      <c r="AA2">
         <v>1240725</v>
       </c>
-      <c r="P2">
+      <c r="AB2">
         <v>510627</v>
       </c>
-      <c r="Q2">
+      <c r="AC2">
         <v>1300712</v>
       </c>
-      <c r="R2">
+      <c r="AD2">
         <v>835410</v>
       </c>
-      <c r="S2">
+      <c r="AE2">
         <v>857241</v>
       </c>
-      <c r="T2">
+      <c r="AF2">
         <v>984571</v>
       </c>
-      <c r="U2">
-        <f>AVERAGE(I2:T2)</f>
+      <c r="AG2">
+        <f>AVERAGE(U2:AF2)</f>
         <v>750262.58333333337</v>
       </c>
-      <c r="V2">
-        <f>U12</f>
+      <c r="AH2">
+        <f>AG12</f>
         <v>1039408.6666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1892,55 +1983,91 @@
         <v>5.37</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C10" si="0">U3*100/V3</f>
+        <f t="shared" ref="C3:C10" si="0">AG3*100/AH3</f>
         <v>20.60043915995826</v>
       </c>
+      <c r="F3">
+        <v>63882</v>
+      </c>
+      <c r="G3">
+        <v>44090</v>
+      </c>
+      <c r="H3">
+        <v>227332</v>
+      </c>
       <c r="I3">
+        <v>148443</v>
+      </c>
+      <c r="J3">
+        <v>45377</v>
+      </c>
+      <c r="K3">
+        <v>101998</v>
+      </c>
+      <c r="L3">
+        <v>112570</v>
+      </c>
+      <c r="M3">
+        <v>231830</v>
+      </c>
+      <c r="N3">
+        <v>258980</v>
+      </c>
+      <c r="O3">
+        <v>114323</v>
+      </c>
+      <c r="P3">
+        <v>133747</v>
+      </c>
+      <c r="Q3">
+        <v>77267</v>
+      </c>
+      <c r="U3">
         <v>106255</v>
       </c>
-      <c r="J3">
+      <c r="V3">
         <v>515944</v>
       </c>
-      <c r="K3">
+      <c r="W3">
         <v>17608</v>
       </c>
-      <c r="L3">
+      <c r="X3">
         <v>77817</v>
       </c>
-      <c r="M3">
+      <c r="Y3">
         <v>155598</v>
       </c>
-      <c r="N3">
+      <c r="Z3">
         <v>82978</v>
       </c>
-      <c r="O3">
+      <c r="AA3">
         <v>557157</v>
       </c>
-      <c r="P3">
+      <c r="AB3">
         <v>68036</v>
       </c>
-      <c r="Q3">
+      <c r="AC3">
         <v>300915</v>
       </c>
-      <c r="R3">
+      <c r="AD3">
         <v>88103</v>
       </c>
-      <c r="S3">
+      <c r="AE3">
         <v>340703</v>
       </c>
-      <c r="T3">
+      <c r="AF3">
         <v>258359</v>
       </c>
-      <c r="U3">
-        <f>AVERAGE(I3:T3)</f>
+      <c r="AG3">
+        <f>AVERAGE(U3:AF3)</f>
         <v>214122.75</v>
       </c>
-      <c r="V3">
-        <f>V2</f>
+      <c r="AH3">
+        <f>AH2</f>
         <v>1039408.6666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1952,52 +2079,88 @@
         <f t="shared" si="0"/>
         <v>5.1154887426376412</v>
       </c>
+      <c r="F4">
+        <v>8248</v>
+      </c>
+      <c r="G4">
+        <v>391357</v>
+      </c>
+      <c r="H4">
+        <v>16506</v>
+      </c>
       <c r="I4">
+        <v>20132</v>
+      </c>
+      <c r="J4">
+        <v>51980</v>
+      </c>
+      <c r="K4">
+        <v>22048</v>
+      </c>
+      <c r="L4">
+        <v>392293</v>
+      </c>
+      <c r="M4">
+        <v>27279</v>
+      </c>
+      <c r="N4">
+        <v>177630</v>
+      </c>
+      <c r="O4">
+        <v>21295</v>
+      </c>
+      <c r="P4">
+        <v>127491</v>
+      </c>
+      <c r="Q4">
+        <v>168199</v>
+      </c>
+      <c r="U4">
         <v>21361</v>
       </c>
-      <c r="J4">
+      <c r="V4">
         <v>91940</v>
       </c>
-      <c r="K4">
+      <c r="W4">
         <v>7983</v>
       </c>
-      <c r="L4">
+      <c r="X4">
         <v>55329</v>
       </c>
-      <c r="M4">
+      <c r="Y4">
         <v>25751</v>
       </c>
-      <c r="N4">
+      <c r="Z4">
         <v>34564</v>
       </c>
-      <c r="O4">
+      <c r="AA4">
         <v>165763</v>
       </c>
-      <c r="P4">
+      <c r="AB4">
         <v>17637</v>
       </c>
-      <c r="Q4">
+      <c r="AC4">
         <v>58696</v>
       </c>
-      <c r="R4">
+      <c r="AD4">
         <v>31731</v>
       </c>
-      <c r="S4">
+      <c r="AE4">
         <v>70266</v>
       </c>
-      <c r="T4">
+      <c r="AF4">
         <v>57029</v>
       </c>
-      <c r="U4">
-        <f t="shared" ref="U4:U10" si="1">AVERAGE(I4:T4)</f>
+      <c r="AG4">
+        <f t="shared" ref="AG4:AG10" si="1">AVERAGE(U4:AF4)</f>
         <v>53170.833333333336</v>
       </c>
-      <c r="V4">
-        <f t="shared" ref="V4:V10" si="2">V3</f>
+      <c r="AH4">
+        <f t="shared" ref="AH4:AH10" si="2">AH3</f>
         <v>1039408.6666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2008,52 +2171,52 @@
         <f t="shared" si="0"/>
         <v>0.58926934737892644</v>
       </c>
-      <c r="I5">
+      <c r="U5">
         <v>12766</v>
       </c>
-      <c r="J5">
+      <c r="V5">
         <v>5357</v>
       </c>
-      <c r="K5">
+      <c r="W5">
         <v>2027</v>
       </c>
-      <c r="L5">
+      <c r="X5">
         <v>8065</v>
       </c>
-      <c r="M5">
+      <c r="Y5">
         <v>4653</v>
       </c>
-      <c r="N5">
+      <c r="Z5">
         <v>5424</v>
       </c>
-      <c r="O5">
+      <c r="AA5">
         <v>8440</v>
       </c>
-      <c r="P5">
+      <c r="AB5">
         <v>6608</v>
       </c>
-      <c r="Q5">
+      <c r="AC5">
         <v>3222</v>
       </c>
-      <c r="R5">
+      <c r="AD5">
         <v>8716</v>
       </c>
-      <c r="S5">
+      <c r="AE5">
         <v>5582</v>
       </c>
-      <c r="T5">
+      <c r="AF5">
         <v>2639</v>
       </c>
-      <c r="U5">
+      <c r="AG5">
         <f t="shared" si="1"/>
         <v>6124.916666666667</v>
       </c>
-      <c r="V5">
+      <c r="AH5">
         <f t="shared" si="2"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2064,52 +2227,52 @@
         <f t="shared" si="0"/>
         <v>0.14167510629441227</v>
       </c>
-      <c r="I6">
+      <c r="U6">
         <v>284</v>
       </c>
-      <c r="J6">
+      <c r="V6">
         <v>3659</v>
       </c>
-      <c r="K6">
+      <c r="W6">
         <v>220</v>
       </c>
-      <c r="L6">
+      <c r="X6">
         <v>1507</v>
       </c>
-      <c r="M6">
+      <c r="Y6">
         <v>1837</v>
       </c>
-      <c r="N6">
+      <c r="Z6">
         <v>97</v>
       </c>
-      <c r="O6">
+      <c r="AA6">
         <v>1376</v>
       </c>
-      <c r="P6">
+      <c r="AB6">
         <v>479</v>
       </c>
-      <c r="Q6">
+      <c r="AC6">
         <v>420</v>
       </c>
-      <c r="R6">
+      <c r="AD6">
         <v>1200</v>
       </c>
-      <c r="S6">
+      <c r="AE6">
         <v>5512</v>
       </c>
-      <c r="T6">
+      <c r="AF6">
         <v>1080</v>
       </c>
-      <c r="U6">
+      <c r="AG6">
         <f t="shared" si="1"/>
         <v>1472.5833333333333</v>
       </c>
-      <c r="V6">
+      <c r="AH6">
         <f t="shared" si="2"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2120,52 +2283,52 @@
         <f t="shared" si="0"/>
         <v>0.13661614007451672</v>
       </c>
-      <c r="I7">
+      <c r="U7">
         <v>172</v>
       </c>
-      <c r="J7">
+      <c r="V7">
         <v>1469</v>
       </c>
-      <c r="K7">
+      <c r="W7">
         <v>266</v>
       </c>
-      <c r="L7">
+      <c r="X7">
         <v>1727</v>
       </c>
-      <c r="M7">
+      <c r="Y7">
         <v>1262</v>
       </c>
-      <c r="N7">
+      <c r="Z7">
         <v>829</v>
       </c>
-      <c r="O7">
+      <c r="AA7">
         <v>2676</v>
       </c>
-      <c r="P7">
+      <c r="AB7">
         <v>1379</v>
       </c>
-      <c r="Q7">
+      <c r="AC7">
         <v>982</v>
       </c>
-      <c r="R7">
+      <c r="AD7">
         <v>1667</v>
       </c>
-      <c r="S7">
+      <c r="AE7">
         <v>2117</v>
       </c>
-      <c r="T7">
+      <c r="AF7">
         <v>2494</v>
       </c>
-      <c r="U7">
+      <c r="AG7">
         <f t="shared" si="1"/>
         <v>1420</v>
       </c>
-      <c r="V7">
+      <c r="AH7">
         <f t="shared" si="2"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2176,52 +2339,52 @@
         <f t="shared" si="0"/>
         <v>1.908937966651551E-2</v>
       </c>
-      <c r="I8">
+      <c r="U8">
         <v>44</v>
       </c>
-      <c r="J8">
+      <c r="V8">
         <v>377</v>
       </c>
-      <c r="K8">
+      <c r="W8">
         <v>18</v>
       </c>
-      <c r="L8">
+      <c r="X8">
         <v>217</v>
       </c>
-      <c r="M8">
+      <c r="Y8">
         <v>113</v>
       </c>
-      <c r="N8">
+      <c r="Z8">
         <v>116</v>
       </c>
-      <c r="O8">
+      <c r="AA8">
         <v>899</v>
       </c>
-      <c r="P8">
+      <c r="AB8">
         <v>17</v>
       </c>
-      <c r="Q8">
+      <c r="AC8">
         <v>115</v>
       </c>
-      <c r="R8">
+      <c r="AD8">
         <v>135</v>
       </c>
-      <c r="S8">
+      <c r="AE8">
         <v>238</v>
       </c>
-      <c r="T8">
+      <c r="AF8">
         <v>92</v>
       </c>
-      <c r="U8">
+      <c r="AG8">
         <f t="shared" si="1"/>
         <v>198.41666666666666</v>
       </c>
-      <c r="V8">
+      <c r="AH8">
         <f t="shared" si="2"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2232,52 +2395,52 @@
         <f t="shared" si="0"/>
         <v>3.8523506634862266E-2</v>
       </c>
-      <c r="I9">
+      <c r="U9">
         <v>38</v>
       </c>
-      <c r="J9">
+      <c r="V9">
         <v>962</v>
       </c>
-      <c r="K9">
+      <c r="W9">
         <v>30</v>
       </c>
-      <c r="L9">
+      <c r="X9">
         <v>67</v>
       </c>
-      <c r="M9">
+      <c r="Y9">
         <v>199</v>
       </c>
-      <c r="N9">
+      <c r="Z9">
         <v>139</v>
       </c>
-      <c r="O9">
+      <c r="AA9">
         <v>1410</v>
       </c>
-      <c r="P9">
+      <c r="AB9">
         <v>81</v>
       </c>
-      <c r="Q9">
+      <c r="AC9">
         <v>787</v>
       </c>
-      <c r="R9">
+      <c r="AD9">
         <v>105</v>
       </c>
-      <c r="S9">
+      <c r="AE9">
         <v>425</v>
       </c>
-      <c r="T9">
+      <c r="AF9">
         <v>562</v>
       </c>
-      <c r="U9">
+      <c r="AG9">
         <f t="shared" si="1"/>
         <v>400.41666666666669</v>
       </c>
-      <c r="V9">
+      <c r="AH9">
         <f t="shared" si="2"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2288,55 +2451,296 @@
         <f t="shared" si="0"/>
         <v>1.1772238445834264</v>
       </c>
-      <c r="I10">
+      <c r="U10">
         <v>23744</v>
       </c>
-      <c r="J10">
+      <c r="V10">
         <v>9821</v>
       </c>
-      <c r="K10">
+      <c r="W10">
         <v>711</v>
       </c>
-      <c r="L10">
+      <c r="X10">
         <v>30920</v>
       </c>
-      <c r="M10">
+      <c r="Y10">
         <v>2440</v>
       </c>
-      <c r="N10">
+      <c r="Z10">
         <v>11627</v>
       </c>
-      <c r="O10">
+      <c r="AA10">
         <v>7634</v>
       </c>
-      <c r="P10">
+      <c r="AB10">
         <v>17760</v>
       </c>
-      <c r="Q10">
+      <c r="AC10">
         <v>20837</v>
       </c>
-      <c r="R10">
+      <c r="AD10">
         <v>3305</v>
       </c>
-      <c r="S10">
+      <c r="AE10">
         <v>4133</v>
       </c>
-      <c r="T10">
+      <c r="AF10">
         <v>13902</v>
       </c>
-      <c r="U10">
+      <c r="AG10">
         <f t="shared" si="1"/>
         <v>12236.166666666666</v>
       </c>
-      <c r="V10">
+      <c r="AH10">
         <f t="shared" si="2"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12">
+        <f>SUM(F2:F4)</f>
+        <v>2236240</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:Q12" si="3">SUM(G2:G4)</f>
+        <v>2857095</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>1332260</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>3102181</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>1997834</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>1538095</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>2948840</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>1677806</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>2539872</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="3"/>
+        <v>2474593</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>4072516</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="3"/>
+        <v>2272177</v>
+      </c>
       <c r="U12">
         <f>SUM(U2:U10)</f>
+        <v>675874</v>
+      </c>
+      <c r="V12">
+        <f t="shared" ref="V12:AF12" si="4">SUM(V2:V10)</f>
+        <v>1249676</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="4"/>
+        <v>349860</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="4"/>
+        <v>1037481</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="4"/>
+        <v>609790</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="4"/>
+        <v>677516</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="4"/>
+        <v>1986080</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="4"/>
+        <v>622624</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="4"/>
+        <v>1686686</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="4"/>
+        <v>970372</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="4"/>
+        <v>1286217</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="4"/>
+        <v>1320728</v>
+      </c>
+      <c r="AG12">
+        <f>SUM(AG2:AG10)</f>
         <v>1039408.6666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13">
+        <v>8985176</v>
+      </c>
+      <c r="G13">
+        <v>11725404</v>
+      </c>
+      <c r="H13">
+        <v>5481988</v>
+      </c>
+      <c r="I13">
+        <v>12540804</v>
+      </c>
+      <c r="J13">
+        <v>8086784</v>
+      </c>
+      <c r="K13">
+        <v>6317488</v>
+      </c>
+      <c r="L13">
+        <v>12350020</v>
+      </c>
+      <c r="M13">
+        <v>6883748</v>
+      </c>
+      <c r="N13">
+        <v>10707296</v>
+      </c>
+      <c r="O13">
+        <v>10089840</v>
+      </c>
+      <c r="P13">
+        <v>16571364</v>
+      </c>
+      <c r="Q13">
+        <v>9383212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <f>F13/4</f>
+        <v>2246294</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:Q14" si="5">G13/4</f>
+        <v>2931351</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>1370497</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>3135201</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="5"/>
+        <v>2021696</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="5"/>
+        <v>1579372</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="5"/>
+        <v>3087505</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="5"/>
+        <v>1720937</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
+        <v>2676824</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="5"/>
+        <v>2522460</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="5"/>
+        <v>4142841</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="5"/>
+        <v>2345803</v>
+      </c>
+      <c r="U14">
+        <f>F14</f>
+        <v>2246294</v>
+      </c>
+      <c r="V14">
+        <f t="shared" ref="V14:AG14" si="6">G14</f>
+        <v>2931351</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="6"/>
+        <v>1370497</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="6"/>
+        <v>3135201</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="6"/>
+        <v>2021696</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="6"/>
+        <v>1579372</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="6"/>
+        <v>3087505</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="6"/>
+        <v>1720937</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="6"/>
+        <v>2676824</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="6"/>
+        <v>2522460</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="6"/>
+        <v>4142841</v>
+      </c>
+      <c r="AF14">
+        <f t="shared" si="6"/>
+        <v>2345803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug found: diamond pp v2 didn't work
v2 now completed.  Refactor went bad
</commit_message>
<xml_diff>
--- a/prototypes/post-run-analysis/taxa_rpk_amalgam/mpro_final_taxa.xlsx
+++ b/prototypes/post-run-analysis/taxa_rpk_amalgam/mpro_final_taxa.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3989EF97-46BD-43F2-AF2B-ECD1507D7F87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9055FDD3-61D9-4453-8D7B-28F25A02B4D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="8370" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>unmapped</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>raw reads</t>
+  </si>
+  <si>
+    <t>humann2 avg</t>
+  </si>
+  <si>
+    <t>total annotated</t>
+  </si>
+  <si>
+    <t>discarded</t>
   </si>
 </sst>
 </file>
@@ -222,11 +231,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>Sheet1!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>unmapped</c:v>
+                  <c:v>discarded</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -243,36 +252,36 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$C$1</c:f>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>humann2 percent</c:v>
+                  <c:v>humann2 avg</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>mpro percentage</c:v>
+                  <c:v>mpro avg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$C$2</c:f>
+              <c:f>Sheet1!$B$19:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>89.72</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72.181674772771458</c:v>
+                  <c:v>1442323.0833333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6E71-4F32-BBFD-04DDDBE854DE}"/>
+              <c16:uniqueId val="{00000000-1E40-43D5-BB47-1166FDD63D45}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -281,70 +290,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>unclassified</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$1:$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>humann2 percent</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>mpro percentage</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$C$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>5.37</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20.60043915995826</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6E71-4F32-BBFD-04DDDBE854DE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>up to species</c:v>
+                  <c:v>unmapped</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -361,108 +311,49 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$C$1</c:f>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>humann2 percent</c:v>
+                  <c:v>humann2 avg</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>mpro percentage</c:v>
+                  <c:v>mpro avg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$C$4</c:f>
+              <c:f>Sheet1!$B$20:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4.910000000000001</c:v>
+                  <c:v>2330984.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1154887426376412</c:v>
+                  <c:v>750262.58333333337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6E71-4F32-BBFD-04DDDBE854DE}"/>
+              <c16:uniqueId val="{00000001-1E40-43D5-BB47-1166FDD63D45}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>Sheet1!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>up to genus</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$1:$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>humann2 percent</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>mpro percentage</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$5:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.58926934737892644</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-6E71-4F32-BBFD-04DDDBE854DE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>up to family</c:v>
+                  <c:v>unclassified</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -479,21 +370,21 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$C$1</c:f>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>humann2 percent</c:v>
+                  <c:v>humann2 avg</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>mpro percentage</c:v>
+                  <c:v>mpro avg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$C$6</c:f>
+              <c:f>Sheet1!$B$21:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -501,86 +392,27 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14167510629441227</c:v>
+                  <c:v>214122.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-6E71-4F32-BBFD-04DDDBE854DE}"/>
+              <c16:uniqueId val="{00000002-1E40-43D5-BB47-1166FDD63D45}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>Sheet1!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>up to order</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$1:$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>humann2 percent</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>mpro percentage</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$7:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.13661614007451672</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-6E71-4F32-BBFD-04DDDBE854DE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>up to class</c:v>
+                  <c:v>up to species</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -599,110 +431,49 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$C$1</c:f>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>humann2 percent</c:v>
+                  <c:v>humann2 avg</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>mpro percentage</c:v>
+                  <c:v>mpro avg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$C$8</c:f>
+              <c:f>Sheet1!$B$22:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>150747</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.908937966651551E-2</c:v>
+                  <c:v>53170.833333333336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-6E71-4F32-BBFD-04DDDBE854DE}"/>
+              <c16:uniqueId val="{00000003-1E40-43D5-BB47-1166FDD63D45}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>Sheet1!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>up to phylum</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$1:$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>humann2 percent</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>mpro percentage</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$9:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.8523506634862266E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-6E71-4F32-BBFD-04DDDBE854DE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>up to kingdom</c:v>
+                  <c:v>up to genus</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -721,21 +492,21 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$C$1</c:f>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>humann2 percent</c:v>
+                  <c:v>humann2 avg</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>mpro percentage</c:v>
+                  <c:v>mpro avg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$C$10</c:f>
+              <c:f>Sheet1!$B$23:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -743,14 +514,322 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1772238445834264</c:v>
+                  <c:v>6124.916666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-6E71-4F32-BBFD-04DDDBE854DE}"/>
+              <c16:uniqueId val="{00000004-1E40-43D5-BB47-1166FDD63D45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>up to family</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>humann2 avg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mpro avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1472.5833333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-1E40-43D5-BB47-1166FDD63D45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>up to order</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>humann2 avg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mpro avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$25:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1420</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-1E40-43D5-BB47-1166FDD63D45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>up to class</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>humann2 avg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mpro avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$26:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>198.41666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-1E40-43D5-BB47-1166FDD63D45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>up to phylum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>humann2 avg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mpro avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>400.41666666666669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-1E40-43D5-BB47-1166FDD63D45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>up to kingdom</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>humann2 avg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mpro avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$28:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12236.166666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-1E40-43D5-BB47-1166FDD63D45}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -764,11 +843,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1305221487"/>
-        <c:axId val="1385246079"/>
+        <c:axId val="432449615"/>
+        <c:axId val="422375199"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1305221487"/>
+        <c:axId val="432449615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +890,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1385246079"/>
+        <c:crossAx val="422375199"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -819,7 +898,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1385246079"/>
+        <c:axId val="422375199"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +949,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1305221487"/>
+        <c:crossAx val="432449615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -882,6 +961,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -927,13 +1037,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1475,23 +1582,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1088049</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>73270</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>505558</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>65942</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{953ED075-961E-468C-8C27-A18A6E40C069}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B3298CE-6689-4D95-A2D1-9E0FA0D9474F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1775,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI14"/>
+  <dimension ref="A1:AI28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AG14" sqref="AG14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,6 +1893,7 @@
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="33" max="33" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -1834,6 +1942,9 @@
       <c r="Q1" t="s">
         <v>20</v>
       </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
       <c r="T1" t="s">
         <v>26</v>
       </c>
@@ -1895,40 +2006,52 @@
         <v>72.181674772771458</v>
       </c>
       <c r="F2">
-        <v>2164110</v>
+        <v>2230250</v>
       </c>
       <c r="G2">
-        <v>2421648</v>
+        <v>2464348</v>
       </c>
       <c r="H2">
-        <v>1088422</v>
+        <v>1355386</v>
       </c>
       <c r="I2">
-        <v>2933606</v>
+        <v>3092229</v>
       </c>
       <c r="J2">
-        <v>1900477</v>
+        <f>J15-J4</f>
+        <v>1952349</v>
       </c>
       <c r="K2">
-        <v>1414049</v>
+        <f t="shared" ref="K2:Q2" si="0">K15-K4</f>
+        <v>1548083</v>
       </c>
       <c r="L2">
-        <v>2443977</v>
+        <f t="shared" si="0"/>
+        <v>2616817</v>
       </c>
       <c r="M2">
-        <v>1418697</v>
+        <f t="shared" si="0"/>
+        <v>1665227</v>
       </c>
       <c r="N2">
-        <v>2103262</v>
+        <f t="shared" si="0"/>
+        <v>2452464</v>
       </c>
       <c r="O2">
-        <v>2338975</v>
+        <f t="shared" si="0"/>
+        <v>2479919</v>
       </c>
       <c r="P2">
-        <v>3811278</v>
+        <f t="shared" si="0"/>
+        <v>3969061</v>
       </c>
       <c r="Q2">
-        <v>2026711</v>
+        <f t="shared" si="0"/>
+        <v>2145684</v>
+      </c>
+      <c r="R2">
+        <f>AVERAGE(F2:Q2)</f>
+        <v>2330984.75</v>
       </c>
       <c r="U2">
         <v>511210</v>
@@ -1971,7 +2094,7 @@
         <v>750262.58333333337</v>
       </c>
       <c r="AH2">
-        <f>AG12</f>
+        <f>AG13</f>
         <v>1039408.6666666666</v>
       </c>
     </row>
@@ -1983,44 +2106,11 @@
         <v>5.37</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C10" si="0">AG3*100/AH3</f>
+        <f t="shared" ref="C3:C10" si="1">AG3*100/AH3</f>
         <v>20.60043915995826</v>
       </c>
       <c r="F3">
-        <v>63882</v>
-      </c>
-      <c r="G3">
-        <v>44090</v>
-      </c>
-      <c r="H3">
-        <v>227332</v>
-      </c>
-      <c r="I3">
-        <v>148443</v>
-      </c>
-      <c r="J3">
-        <v>45377</v>
-      </c>
-      <c r="K3">
-        <v>101998</v>
-      </c>
-      <c r="L3">
-        <v>112570</v>
-      </c>
-      <c r="M3">
-        <v>231830</v>
-      </c>
-      <c r="N3">
-        <v>258980</v>
-      </c>
-      <c r="O3">
-        <v>114323</v>
-      </c>
-      <c r="P3">
-        <v>133747</v>
-      </c>
-      <c r="Q3">
-        <v>77267</v>
+        <v>0</v>
       </c>
       <c r="U3">
         <v>106255</v>
@@ -2076,44 +2166,59 @@
         <v>4.910000000000001</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1154887426376412</v>
       </c>
       <c r="F4">
-        <v>8248</v>
+        <v>16044</v>
       </c>
       <c r="G4">
-        <v>391357</v>
+        <f>36473+7213+2401+14763+406153</f>
+        <v>467003</v>
       </c>
       <c r="H4">
-        <v>16506</v>
+        <f>15111</f>
+        <v>15111</v>
       </c>
       <c r="I4">
-        <v>20132</v>
+        <f>13160+29812</f>
+        <v>42972</v>
       </c>
       <c r="J4">
-        <v>51980</v>
+        <f>2470+66877</f>
+        <v>69347</v>
       </c>
       <c r="K4">
-        <v>22048</v>
+        <f>30600+667+22</f>
+        <v>31289</v>
       </c>
       <c r="L4">
-        <v>392293</v>
+        <f>401383+12099+1629+6+45027+10542+2</f>
+        <v>470688</v>
       </c>
       <c r="M4">
-        <v>27279</v>
+        <f>25712+1104+28894</f>
+        <v>55710</v>
       </c>
       <c r="N4">
-        <v>177630</v>
+        <f>5278+52296+9+697+5776+160304</f>
+        <v>224360</v>
       </c>
       <c r="O4">
-        <v>21295</v>
+        <f>31820+10721</f>
+        <v>42541</v>
       </c>
       <c r="P4">
-        <v>127491</v>
+        <f>16000+19+7109+150652</f>
+        <v>173780</v>
       </c>
       <c r="Q4">
-        <v>168199</v>
+        <f>3+4549+39780+6+1723+7062+146996</f>
+        <v>200119</v>
+      </c>
+      <c r="R4">
+        <f>AVERAGE(F4:Q4)</f>
+        <v>150747</v>
       </c>
       <c r="U4">
         <v>21361</v>
@@ -2152,11 +2257,11 @@
         <v>57029</v>
       </c>
       <c r="AG4">
-        <f t="shared" ref="AG4:AG10" si="1">AVERAGE(U4:AF4)</f>
+        <f t="shared" ref="AG4:AG10" si="2">AVERAGE(U4:AF4)</f>
         <v>53170.833333333336</v>
       </c>
       <c r="AH4">
-        <f t="shared" ref="AH4:AH10" si="2">AH3</f>
+        <f t="shared" ref="AH4:AH10" si="3">AH3</f>
         <v>1039408.6666666666</v>
       </c>
     </row>
@@ -2168,7 +2273,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.58926934737892644</v>
       </c>
       <c r="U5">
@@ -2208,11 +2313,11 @@
         <v>2639</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6124.916666666667</v>
       </c>
       <c r="AH5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
@@ -2224,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14167510629441227</v>
       </c>
       <c r="U6">
@@ -2264,11 +2369,11 @@
         <v>1080</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1472.5833333333333</v>
       </c>
       <c r="AH6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
@@ -2280,7 +2385,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13661614007451672</v>
       </c>
       <c r="U7">
@@ -2320,11 +2425,11 @@
         <v>2494</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1420</v>
       </c>
       <c r="AH7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
@@ -2336,7 +2441,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.908937966651551E-2</v>
       </c>
       <c r="U8">
@@ -2376,11 +2481,11 @@
         <v>92</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>198.41666666666666</v>
       </c>
       <c r="AH8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
@@ -2392,7 +2497,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8523506634862266E-2</v>
       </c>
       <c r="U9">
@@ -2432,11 +2537,11 @@
         <v>562</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>400.41666666666669</v>
       </c>
       <c r="AH9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1039408.6666666666</v>
       </c>
     </row>
@@ -2448,7 +2553,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1772238445834264</v>
       </c>
       <c r="U10">
@@ -2488,259 +2593,623 @@
         <v>13902</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12236.166666666666</v>
       </c>
       <c r="AH10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1039408.6666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <f>SUM(F4:F10)</f>
+        <v>16044</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:R11" si="4">SUM(G4:G10)</f>
+        <v>467003</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>15111</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>42972</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>69347</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>31289</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>470688</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>55710</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>224360</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="4"/>
+        <v>42541</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>173780</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="4"/>
+        <v>200119</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="4"/>
+        <v>150747</v>
+      </c>
+      <c r="U11">
+        <f>SUM(U4:U10)</f>
+        <v>58409</v>
+      </c>
+      <c r="V11">
+        <f t="shared" ref="V11:AG11" si="5">SUM(V4:V10)</f>
+        <v>113585</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="5"/>
+        <v>11255</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="5"/>
+        <v>97832</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="5"/>
+        <v>36255</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="5"/>
+        <v>52796</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="5"/>
+        <v>188198</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="5"/>
+        <v>43961</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="5"/>
+        <v>85059</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="5"/>
+        <v>46859</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="5"/>
+        <v>88273</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="5"/>
+        <v>77798</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="5"/>
+        <v>75023.333333333328</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F12">
-        <f>SUM(F2:F4)</f>
-        <v>2236240</v>
+        <f>F13-F15</f>
+        <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" ref="G12:Q12" si="3">SUM(G2:G4)</f>
-        <v>2857095</v>
+        <f t="shared" ref="G12:Q12" si="6">G13-G15</f>
+        <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="3"/>
-        <v>1332260</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
-        <v>3102181</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" si="3"/>
-        <v>1997834</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
-        <v>1538095</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="L12">
-        <f t="shared" si="3"/>
-        <v>2948840</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="3"/>
-        <v>1677806</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="N12">
-        <f t="shared" si="3"/>
-        <v>2539872</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" si="3"/>
-        <v>2474593</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="P12">
-        <f t="shared" si="3"/>
-        <v>4072516</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="3"/>
-        <v>2272177</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="U12">
-        <f>SUM(U2:U10)</f>
-        <v>675874</v>
+        <f>U15-U13</f>
+        <v>1570420</v>
       </c>
       <c r="V12">
-        <f t="shared" ref="V12:AF12" si="4">SUM(V2:V10)</f>
-        <v>1249676</v>
+        <f t="shared" ref="V12:AG12" si="7">V15-V13</f>
+        <v>1681675</v>
       </c>
       <c r="W12">
-        <f t="shared" si="4"/>
-        <v>349860</v>
+        <f t="shared" si="7"/>
+        <v>1020637</v>
       </c>
       <c r="X12">
-        <f t="shared" si="4"/>
-        <v>1037481</v>
+        <f t="shared" si="7"/>
+        <v>2097720</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="4"/>
-        <v>609790</v>
+        <f t="shared" si="7"/>
+        <v>1411906</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="4"/>
-        <v>677516</v>
+        <f t="shared" si="7"/>
+        <v>901856</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="4"/>
-        <v>1986080</v>
+        <f t="shared" si="7"/>
+        <v>1101425</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="4"/>
-        <v>622624</v>
+        <f t="shared" si="7"/>
+        <v>1098313</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="4"/>
-        <v>1686686</v>
+        <f t="shared" si="7"/>
+        <v>990138</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="4"/>
-        <v>970372</v>
+        <f t="shared" si="7"/>
+        <v>1552088</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="4"/>
-        <v>1286217</v>
+        <f t="shared" si="7"/>
+        <v>2856624</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="4"/>
-        <v>1320728</v>
+        <f t="shared" si="7"/>
+        <v>1025075</v>
       </c>
       <c r="AG12">
-        <f>SUM(AG2:AG10)</f>
-        <v>1039408.6666666666</v>
+        <f t="shared" si="7"/>
+        <v>1442323.0833333335</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F13">
-        <v>8985176</v>
+        <f>SUM(F2:F4)</f>
+        <v>2246294</v>
       </c>
       <c r="G13">
-        <v>11725404</v>
+        <f t="shared" ref="G13:R13" si="8">SUM(G2:G4)</f>
+        <v>2931351</v>
       </c>
       <c r="H13">
-        <v>5481988</v>
+        <f t="shared" si="8"/>
+        <v>1370497</v>
       </c>
       <c r="I13">
-        <v>12540804</v>
+        <f t="shared" si="8"/>
+        <v>3135201</v>
       </c>
       <c r="J13">
-        <v>8086784</v>
+        <f t="shared" si="8"/>
+        <v>2021696</v>
       </c>
       <c r="K13">
-        <v>6317488</v>
+        <f t="shared" si="8"/>
+        <v>1579372</v>
       </c>
       <c r="L13">
-        <v>12350020</v>
+        <f t="shared" si="8"/>
+        <v>3087505</v>
       </c>
       <c r="M13">
-        <v>6883748</v>
+        <f t="shared" si="8"/>
+        <v>1720937</v>
       </c>
       <c r="N13">
-        <v>10707296</v>
+        <f t="shared" si="8"/>
+        <v>2676824</v>
       </c>
       <c r="O13">
-        <v>10089840</v>
+        <f t="shared" si="8"/>
+        <v>2522460</v>
       </c>
       <c r="P13">
-        <v>16571364</v>
+        <f t="shared" si="8"/>
+        <v>4142841</v>
       </c>
       <c r="Q13">
-        <v>9383212</v>
+        <f t="shared" si="8"/>
+        <v>2345803</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="8"/>
+        <v>2481731.75</v>
+      </c>
+      <c r="U13">
+        <f>SUM(U2:U10)</f>
+        <v>675874</v>
+      </c>
+      <c r="V13">
+        <f t="shared" ref="V13:AF13" si="9">SUM(V2:V10)</f>
+        <v>1249676</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="9"/>
+        <v>349860</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="9"/>
+        <v>1037481</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="9"/>
+        <v>609790</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="9"/>
+        <v>677516</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="9"/>
+        <v>1986080</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="9"/>
+        <v>622624</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="9"/>
+        <v>1686686</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="9"/>
+        <v>970372</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="9"/>
+        <v>1286217</v>
+      </c>
+      <c r="AF13">
+        <f t="shared" si="9"/>
+        <v>1320728</v>
+      </c>
+      <c r="AG13">
+        <f>SUM(AG2:AG10)</f>
+        <v>1039408.6666666666</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14">
+        <v>8985176</v>
+      </c>
+      <c r="G14">
+        <v>11725404</v>
+      </c>
+      <c r="H14">
+        <v>5481988</v>
+      </c>
+      <c r="I14">
+        <v>12540804</v>
+      </c>
+      <c r="J14">
+        <v>8086784</v>
+      </c>
+      <c r="K14">
+        <v>6317488</v>
+      </c>
+      <c r="L14">
+        <v>12350020</v>
+      </c>
+      <c r="M14">
+        <v>6883748</v>
+      </c>
+      <c r="N14">
+        <v>10707296</v>
+      </c>
+      <c r="O14">
+        <v>10089840</v>
+      </c>
+      <c r="P14">
+        <v>16571364</v>
+      </c>
+      <c r="Q14">
+        <v>9383212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="F14">
-        <f>F13/4</f>
+      <c r="F15">
+        <f>F14/4</f>
         <v>2246294</v>
       </c>
-      <c r="G14">
-        <f t="shared" ref="G14:Q14" si="5">G13/4</f>
+      <c r="G15">
+        <f t="shared" ref="G15:Q15" si="10">G14/4</f>
         <v>2931351</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="5"/>
+      <c r="H15">
+        <f t="shared" si="10"/>
         <v>1370497</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="5"/>
+      <c r="I15">
+        <f t="shared" si="10"/>
         <v>3135201</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="5"/>
+      <c r="J15">
+        <f t="shared" si="10"/>
         <v>2021696</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="5"/>
+      <c r="K15">
+        <f t="shared" si="10"/>
         <v>1579372</v>
       </c>
-      <c r="L14">
-        <f t="shared" si="5"/>
+      <c r="L15">
+        <f t="shared" si="10"/>
         <v>3087505</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="5"/>
+      <c r="M15">
+        <f t="shared" si="10"/>
         <v>1720937</v>
       </c>
-      <c r="N14">
-        <f t="shared" si="5"/>
+      <c r="N15">
+        <f t="shared" si="10"/>
         <v>2676824</v>
       </c>
-      <c r="O14">
-        <f t="shared" si="5"/>
+      <c r="O15">
+        <f t="shared" si="10"/>
         <v>2522460</v>
       </c>
-      <c r="P14">
-        <f t="shared" si="5"/>
+      <c r="P15">
+        <f t="shared" si="10"/>
         <v>4142841</v>
       </c>
-      <c r="Q14">
-        <f t="shared" si="5"/>
+      <c r="Q15">
+        <f t="shared" si="10"/>
         <v>2345803</v>
       </c>
-      <c r="U14">
-        <f>F14</f>
+      <c r="R15">
+        <f>AVERAGE(F15:Q15)</f>
+        <v>2481731.75</v>
+      </c>
+      <c r="U15">
+        <f>F15</f>
         <v>2246294</v>
       </c>
-      <c r="V14">
-        <f t="shared" ref="V14:AG14" si="6">G14</f>
+      <c r="V15">
+        <f t="shared" ref="V15:AF15" si="11">G15</f>
         <v>2931351</v>
       </c>
-      <c r="W14">
-        <f t="shared" si="6"/>
+      <c r="W15">
+        <f t="shared" si="11"/>
         <v>1370497</v>
       </c>
-      <c r="X14">
-        <f t="shared" si="6"/>
+      <c r="X15">
+        <f t="shared" si="11"/>
         <v>3135201</v>
       </c>
-      <c r="Y14">
-        <f t="shared" si="6"/>
+      <c r="Y15">
+        <f t="shared" si="11"/>
         <v>2021696</v>
       </c>
-      <c r="Z14">
-        <f t="shared" si="6"/>
+      <c r="Z15">
+        <f t="shared" si="11"/>
         <v>1579372</v>
       </c>
-      <c r="AA14">
-        <f t="shared" si="6"/>
+      <c r="AA15">
+        <f t="shared" si="11"/>
         <v>3087505</v>
       </c>
-      <c r="AB14">
-        <f t="shared" si="6"/>
+      <c r="AB15">
+        <f t="shared" si="11"/>
         <v>1720937</v>
       </c>
-      <c r="AC14">
-        <f t="shared" si="6"/>
+      <c r="AC15">
+        <f t="shared" si="11"/>
         <v>2676824</v>
       </c>
-      <c r="AD14">
-        <f t="shared" si="6"/>
+      <c r="AD15">
+        <f t="shared" si="11"/>
         <v>2522460</v>
       </c>
-      <c r="AE14">
-        <f t="shared" si="6"/>
+      <c r="AE15">
+        <f t="shared" si="11"/>
         <v>4142841</v>
       </c>
-      <c r="AF14">
-        <f t="shared" si="6"/>
+      <c r="AF15">
+        <f t="shared" si="11"/>
         <v>2345803</v>
+      </c>
+      <c r="AG15">
+        <f>AVERAGE(U15:AF15)</f>
+        <v>2481731.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f>AG12</f>
+        <v>1442323.0833333335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:B28" si="12">R2</f>
+        <v>2330984.75</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:C28" si="13">AG2</f>
+        <v>750262.58333333337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="13"/>
+        <v>214122.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="12"/>
+        <v>150747</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="13"/>
+        <v>53170.833333333336</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="13"/>
+        <v>6124.916666666667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="13"/>
+        <v>1472.5833333333333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="13"/>
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="13"/>
+        <v>198.41666666666666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="13"/>
+        <v>400.41666666666669</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="13"/>
+        <v>12236.166666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>